<commit_message>
commit to update the communication style dictionary
</commit_message>
<xml_diff>
--- a/style_dict.xlsx
+++ b/style_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinchenxie/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C1DEE95-14C9-0E41-B223-EE3BB3F0A25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD938C7-1C1C-B34E-82C0-248610CEA48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="12960" windowWidth="28040" windowHeight="17440" xr2:uid="{7BB58C95-B7E8-B642-94E0-75D665E71FD5}"/>
+    <workbookView xWindow="6520" yWindow="4900" windowWidth="28040" windowHeight="17440" xr2:uid="{7BB58C95-B7E8-B642-94E0-75D665E71FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>style</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,14 +56,76 @@
     <t>Authoritative is the tendency to command or demand others in a conversation, without considering the others' willingness and concerns.</t>
   </si>
   <si>
-    <t xml:space="preserve">I am not very likely to tell someone what they should do; I sometimes insist that otheres do what I say; I expect people to obey when I ask them to do something; When I feel others should do something for me, I ask for it in a demanding tone of voice. </t>
+    <t>Talkativeness is a tendency to initiate a conversation, talk a lot, and avoid silence in a conversation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talkative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>informality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Informality is a tendency to talk casually and avoid being formal, distant, or stiff in a conversation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">I am very likely to tell someone what they should do; I sometimes insist that otheres do what I say; I expect people to obey when I ask them to do something; When I feel others should do something for me, I ask for it in a demanding tone of voice. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I always have a lot to say; I have a hard time keeping myself silent when around other people; I am always the one who breaks a silence by starting to talk; I like to talk a lot.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sentimentality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sentimentality is a tendency to express one's own emotions or display empathic emotional responses to others in a conversation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">I never communicate with others in a distant manner; I never behave formally when I meet someone; I always address others in a very casual way; I never come across as somewhat stiff when dealing with people.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conciseness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conciseness is the tendency to use as few words as possible to clearly convey ideas and explain things in a conversation, and avoid being long-winded.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I don’t need a lot of words to get my message across; Most of the time, I only need a few words to explain something; With a few words I can usually clarify my point to everybody.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When I see others cry, I have difficulty holding back my tears; During a conversation, I am easily overcome by emotions; When describing my memories, i sometimes get visibily emotional; People can tell that I am emotionally touched by some topics of conversation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conversational dominance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conversational dominance is the tendency to take the lead in a conversation and detremine its topics and directions.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I often take the lead in a conversation; I often determine which topics are talked about during a conversation; I often determine the direction of a conversation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -81,8 +143,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFA31515"/>
-      <name val="Menlo"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -108,12 +175,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,34 +525,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD60F556-46FC-5E43-8515-B00E69352796}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="83.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="169" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="68">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>